<commit_message>
about section ainda por melhorar, e inserir video de demonstraçao
</commit_message>
<xml_diff>
--- a/assets/Documents/Calendário.xlsx
+++ b/assets/Documents/Calendário.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26516"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João\Desktop\ECI-3ano\PECI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A12A62B-9BD2-4B9D-97DB-FCC397BAEA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3196A54E-311F-42B7-BDB4-A3A0BCD30EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>PECI 21/22 - GRUPO 11</t>
   </si>
@@ -142,7 +155,7 @@
     <t>Discussão e definição da arquitetura do sistema</t>
   </si>
   <si>
-    <t>Definição e criação das bases de dados</t>
+    <t>Definição e criação da bases de dados</t>
   </si>
   <si>
     <t>Especificação da API</t>
@@ -151,19 +164,22 @@
     <t xml:space="preserve">Criação da API </t>
   </si>
   <si>
-    <t>Criação da página do stakeholder</t>
+    <t>Criação da página do stakeholder - Área da Empresa</t>
+  </si>
+  <si>
+    <t>Registo das Empresas</t>
+  </si>
+  <si>
+    <t>Criação de Anúncios</t>
+  </si>
+  <si>
+    <t>Visualização de Anúncios por parte dos clientes</t>
   </si>
   <si>
     <t>Implementação de sistemas de segurança</t>
   </si>
   <si>
-    <t>Design de UI/UX</t>
-  </si>
-  <si>
     <t>Implementação de  um protótipo da plataforma</t>
-  </si>
-  <si>
-    <t>Validação e realização de testes</t>
   </si>
   <si>
     <t>Escrita de documentação de apoio</t>
@@ -188,7 +204,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +250,26 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF70AD47"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFD966"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -314,12 +350,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF833C0C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9E1F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -344,7 +374,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFED7D31"/>
+        <fgColor rgb="FF70AD47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -495,35 +531,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -539,14 +585,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -934,50 +980,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="S28" sqref="S28:T28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="68" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.109375" customWidth="1"/>
-    <col min="17" max="17" width="16.88671875" customWidth="1"/>
-    <col min="18" max="18" width="17.88671875" customWidth="1"/>
-    <col min="19" max="19" width="17.44140625" customWidth="1"/>
-    <col min="20" max="20" width="19.5546875" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="40" t="s">
+    <row r="1" spans="1:21" ht="15.6">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43" t="s">
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
       <c r="P1" s="18" t="s">
         <v>5</v>
       </c>
@@ -997,8 +1043,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="40"/>
+    <row r="2" spans="1:21" ht="15.6">
+      <c r="B2" s="48"/>
       <c r="C2" s="14" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1091,7 @@
       <c r="T2" s="16"/>
       <c r="U2" s="17"/>
     </row>
-    <row r="3" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15.6">
       <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1069,7 +1115,7 @@
       <c r="T3" s="13"/>
       <c r="U3" s="13"/>
     </row>
-    <row r="4" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="13.5" customHeight="1">
       <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
@@ -1077,8 +1123,8 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1093,7 +1139,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21">
       <c r="B5" s="10" t="s">
         <v>26</v>
       </c>
@@ -1107,8 +1153,8 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="42"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -1117,7 +1163,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21">
       <c r="B6" s="7" t="s">
         <v>27</v>
       </c>
@@ -1141,7 +1187,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21">
       <c r="B7" s="7" t="s">
         <v>28</v>
       </c>
@@ -1165,7 +1211,7 @@
       <c r="T7" s="9"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21">
       <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1189,33 +1235,33 @@
       <c r="T8" s="2"/>
       <c r="U8" s="9"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
+    <row r="9" spans="1:21">
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:21" ht="15.6">
+      <c r="A10" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="13"/>
@@ -1238,15 +1284,15 @@
       <c r="T10" s="20"/>
       <c r="U10" s="13"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="33">
+    <row r="11" spans="1:21" ht="15">
+      <c r="A11" s="29">
         <v>1</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="21"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1265,19 +1311,19 @@
       <c r="T11" s="5"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="33">
+    <row r="12" spans="1:21">
+      <c r="A12" s="29">
         <v>2</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="27" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1292,19 +1338,19 @@
       <c r="T12" s="5"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="34">
+    <row r="13" spans="1:21">
+      <c r="A13" s="30">
         <v>3</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="27" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1319,19 +1365,19 @@
       <c r="T13" s="5"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="34">
+    <row r="14" spans="1:21">
+      <c r="A14" s="30">
         <v>4</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="28" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="12"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1346,19 +1392,19 @@
       <c r="T14" s="5"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="34">
+    <row r="15" spans="1:21">
+      <c r="A15" s="30">
         <v>5</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="28" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
       <c r="I15" s="12"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1373,25 +1419,25 @@
       <c r="T15" s="5"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="29">
+    <row r="16" spans="1:21">
+      <c r="A16" s="25">
         <v>6</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="27" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -1400,11 +1446,11 @@
       <c r="T16" s="5"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" s="29">
+    <row r="17" spans="1:21" ht="15">
+      <c r="A17" s="25">
         <v>7</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="27" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="2"/>
@@ -1412,26 +1458,26 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="5"/>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" s="29">
+    <row r="18" spans="1:21">
+      <c r="A18" s="25">
         <v>8</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="27" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="2"/>
@@ -1439,13 +1485,13 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -1454,11 +1500,11 @@
       <c r="T18" s="5"/>
       <c r="U18" s="2"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="29">
+    <row r="19" spans="1:21" ht="15">
+      <c r="A19" s="25">
         <v>9</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="27" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="2"/>
@@ -1470,22 +1516,22 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="5"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="39"/>
+      <c r="T19" s="41"/>
       <c r="U19" s="2"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" s="29">
+    <row r="20" spans="1:21">
+      <c r="A20" s="25">
         <v>10</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="27" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="2"/>
@@ -1497,22 +1543,22 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="5"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="43"/>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A21" s="29">
+    <row r="21" spans="1:21">
+      <c r="A21" s="25">
         <v>11</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="27" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="2"/>
@@ -1524,22 +1570,22 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="2"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" s="29">
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="43"/>
+      <c r="U21" s="12"/>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="25">
         <v>12</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="27" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="2"/>
@@ -1551,22 +1597,22 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="2"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A23" s="29">
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="39"/>
+      <c r="S22" s="39"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="12"/>
+    </row>
+    <row r="23" spans="1:21" ht="15">
+      <c r="A23" s="25">
         <v>13</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="38" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="2"/>
@@ -1578,25 +1624,25 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="35"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="33"/>
+      <c r="T23" s="43"/>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" s="29">
+    <row r="24" spans="1:21" ht="15">
+      <c r="A24" s="37">
         <v>14</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1610,20 +1656,19 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="2"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="29">
+      <c r="Q24" s="12"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="12"/>
+    </row>
+    <row r="25" spans="1:21" ht="15">
+      <c r="A25" s="37">
         <v>15</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1637,14 +1682,14 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
-      <c r="T25" s="35"/>
-      <c r="U25" s="2"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A26" s="29">
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="33"/>
+      <c r="U25" s="12"/>
+    </row>
+    <row r="26" spans="1:21" ht="15">
+      <c r="A26" s="25">
         <v>16</v>
       </c>
       <c r="B26" s="31" t="s">
@@ -1662,79 +1707,108 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="2"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A27" s="29">
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="33"/>
+      <c r="U26" s="12"/>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="25">
         <v>17</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="27" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="35"/>
-      <c r="U27" s="35"/>
-    </row>
-    <row r="28" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="33"/>
+      <c r="U27" s="12"/>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="25">
+        <v>18</v>
+      </c>
       <c r="B28" s="27" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="33"/>
+      <c r="U28" s="12"/>
+    </row>
+    <row r="29" spans="1:21" ht="33.75" customHeight="1">
+      <c r="B29" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37" t="s">
+      <c r="C29" s="2"/>
+      <c r="D29" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="38" t="s">
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="Q28" s="38"/>
-      <c r="R28" s="38"/>
-      <c r="S28" s="38"/>
-      <c r="T28" s="39" t="s">
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="U28" s="39"/>
-    </row>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="U29" s="47"/>
+    </row>
+    <row r="30" spans="1:21" ht="15"/>
+    <row r="31" spans="1:21" ht="15"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="I28:O28"/>
-    <mergeCell ref="P28:S28"/>
-    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="I29:O29"/>
+    <mergeCell ref="P29:S29"/>
+    <mergeCell ref="T29:U29"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="M5:N5"/>

</xml_diff>